<commit_message>
can now add universal columns to init sheet
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/seed_workshop_v002.xlsx
+++ b/excel2sbol/tests/test_files/seed_workshop_v002.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7600" uniqueCount="7505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7597" uniqueCount="7508">
   <si>
     <t>SEVA</t>
   </si>
@@ -22542,49 +22542,58 @@
     <t>";"</t>
   </si>
   <si>
-    <t>LamR</t>
-  </si>
-  <si>
-    <t>TER1</t>
-  </si>
-  <si>
-    <t>LacI Coding Sequence from Potvin-Trottier pLPT119, no stop codon</t>
-  </si>
-  <si>
-    <t>lambdaR Coding Sequence from Potvin-Trottier pLPT119, no stop codon</t>
-  </si>
-  <si>
-    <t>rrnB T1 terminator from Potvin-Trottier pLPT119, extra stop codon</t>
-  </si>
-  <si>
-    <t>gtccatggtgaatgtgaaaccagtaacgttatacgatgtcgcagagtatgccggtgtctcttatcagaccgtttcccgcgtggtgaaccaggccagccacgtttctgcgaaaacgcgggaaaaagtggaagcggcgatggcggagctgaattacattcccaaccgcgtggcacaacaactggcgggcaaacagtcgttgctgattggcgttgccacctccagtctggccctgcacgcgccgtcgcaaattgtcgcggcgattaaatctcgcgccgatcaactgggtgccagcgtggtggtgtcgatggtagaacgaagcggcgtcgaagcctgtaaagcggcggtgcacaatcttctcgcgcaacgcgtcagtgggctgatcattaactatccgctggatgaccaggatgccattgctgtggaagctgcctgcactaatgttccggcgttatttcttgatgtctctgaccagacacccatcaacagtattattttctcccatgaagacggtacgcgactgggcgtggagcatctggtcgcattgggtcaccagcaaatcgcgctgttagcgggcccattaagttctgtctcggcgcgtctgcgtctggctggctggcataaatatctcactcgcaatcaaattcagccgatagcggaacgggaaggcgactggagtgccatgtccggttttcaacaaaccatgcaaatgctgaatgagggcatcgttcccactgcgatgctggttgccaacgatcagatggcgctgggcgcaatgcgcgccattaccgagtccgggctgcgcgttggtgcggatatctcggtagtgggatacgacgataccgaagacagctcatgttatatcccgccgttaaccaccatcaaacaggattttcgcctgctggggcaaaccagcgtggaccgcttgctgcaactctctcagggccaggcggtgaagggcaatcagctgttgcccgtctcactggtgaaaagaaaaaccaccctggcgcccaatacgcaaaccgcctctccccgcgcgttggccgattcattaatgcagctggcacgacaggtttcccgactggaaagcgggcagggctcg</t>
-  </si>
-  <si>
-    <t>gtccctcggtaccaaattccagaaaagaggcctcccgaaaggggggccttttttcgttttggtccgtgcctactctggaaaatcttccctatcagtgatagagattgacatccctatcagtgatagagatactgagcacatcagcaggacgcactgaccagctgtcaccggatgtgctttccggtctgatgagtccgtgaggacgaaacagcctctacaaataattttgtttaaggctcg</t>
-  </si>
-  <si>
-    <t>gtccatttgtcctactcaggagagcgttcaccgacaaacaacagataaaacgaaaggcccagtctttcgactgagcctttcgttttatttgtaaggctcg</t>
-  </si>
-  <si>
-    <t>LacI Potvin</t>
-  </si>
-  <si>
-    <t>restriction pLac</t>
-  </si>
-  <si>
-    <t>pLac promoter with restriction site added</t>
-  </si>
-  <si>
-    <t>restriction BBa_B0015</t>
-  </si>
-  <si>
-    <t>BBa_B0015 with restriction site added</t>
-  </si>
-  <si>
-    <t>gaattcaaaagatctctggcacgacaggtttcccgactggaaagcgggcagtgagcgcaacgcaattaatgtgagttagctcactcattaggcaccccaggctttacactttatgcttccggctcgtatgttgtgtggaattgtgagcggataacaa</t>
-  </si>
-  <si>
-    <t>ccaggcatcaaataaaacgaaaggctcagtcgaaagactgggcctttcgttttatctgttgtttgtcggtgaacgctctctactagagtcacactggctcaccttcgggtgggcctttctgcgtttataggatccaaactcgag</t>
+    <t>RFP</t>
+  </si>
+  <si>
+    <t>CFP</t>
+  </si>
+  <si>
+    <t>GFP-like fluorescent chromoprotein FP538</t>
+  </si>
+  <si>
+    <t>UniProt</t>
+  </si>
+  <si>
+    <t>Uniprot</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/Q9U6Y4</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot</t>
+  </si>
+  <si>
+    <t>https://www.uniprot.org/uniprot/{REPLACE_HERE}</t>
+  </si>
+  <si>
+    <t>UniProt:Q9U6Y4</t>
+  </si>
+  <si>
+    <t>Q9U6Y4</t>
+  </si>
+  <si>
+    <t>YFP</t>
+  </si>
+  <si>
+    <t>Red fluorescent protein eqFP611</t>
+  </si>
+  <si>
+    <t>Q8ISF8</t>
+  </si>
+  <si>
+    <t>Cyan fluorescent protein C1</t>
+  </si>
+  <si>
+    <t>Q66ND6</t>
+  </si>
+  <si>
+    <t>GAGTTGAGTTTCTCGACTTCAGTTGTATCAATTTTGGGGCATCAAGCGATCTATTTTCAACATGGCTCATTCAAAGCACGGTCTAAAAGAAGAAATGACAATGAAATACCACATGGAAGGGTGCGTCAACGGACATAAATTTGTGATCACGGGCGAAGGCATTGGATATCCGTTCAAAGGGAAACAGACTATTAATCTGTGTGTGATCGAAGGGGGACCATTGCCATTTTCCGAAGACATATTGTCAGCTGGCTTTAAGTACGGAGACAGGATTTTCACTGAATATCCTCAAGACATAGTAGACTATTTCAAGAACTCGTGTCCTGCTGGATATACATGGGGCAGGTCTTTTCTCTTTGAGGATGGAGCAGTCTGCATATGCAATGTAGATATAACAGTGAGTGTCAAAGAAAACTGCATTTATCATAAGAGCATATTTAATGGAATGAATTTTCCTGCTGATGGACCTGTGATGAAAAAGATGACAACTAACTGGGAAGCATCCTGCGAGAAGATCATGCCAGTACCTAAGCAGGGGATACTGAAAGGGGATGTCTCCATGTACCTCCTTCTGAAGGATGGTGGGCGTTACCGGTGCCAGTTCGACACAGTTTACAAAGCAAAGTCTGTGCCAAGTAAGATGCCGGAGTGGCACTTCATCCAGCATAAGCTCCTCCGTGAAGACCGCAGCGATGCTAAGAATCAGAAGTGGCAGCTGACAGAGCATGCTATTGCATTCCCTTCTGCCTTGGCCTGATAAGAATGTAGTTCCAACATTTTAATGCATGTGCTTGTCAATTATTCTGATAAAAATGTAGTTGAGTTGAAAACAGACAAGTACAAATAAAGCACATGTAAATCGTCT</t>
+  </si>
+  <si>
+    <t>ATGAATTCACTGATCAAGGAAAATATGCGTATGATGGTGGTCATGGAAGGTTCGGTCAACGGCTACCAATTCAAATGCACAGGTGAAGGAGATGGCAATCCATACATGGGAACTCAAACCATGAGGATCAAAGTCGTCGAGGGAGGACCTCTGCCATTTGCCTTTGACATTCTTGCCACAAGCTTCATGTATGGCAGCAAGACTTTTATCAAGCACACTAAAGGCATTCCTGATTTCTTTAAACAGTCCTTTCCTGAGGGTTTTACTTGGGAAAGAGTTACAAGATACGAAGATGGTGGAGTCTTTACCGTTATGCAGGACACCAGCCTTGAAGATGGCTGTCTCGTTTACCACGCCAAAGTCACTGGGGTAAACTTTCCCTCCAATGGTGCCGTGATGCAGAAGAAGACCAAGGGTTGGGAGCCAAATACAGAGATGCTGTATCCAGCAGATGGTGGTCTGAGGGGATACTCTCAAATGGCACTGAATGTTGATGGTGGTGGCTATCTGTCTTGCTCTTTCGAAACAACTTACAGGTCAAAAAAGACCGTCGAGAACTTCAAGATGCCCGGTTTCCATTTTGTTGATCACCGCCTGGAAAGGTTAGAGGAAAGTGACAAGGAAATGTTCGTAGTACAACACGAACACGCAGTTGCCAAGTTCTGTGACCTTCCATCCAAACTGGGACGTCTTTGA</t>
+  </si>
+  <si>
+    <t>CAGTTTCAGTCAGTAACGGTCAGGGACGGTCAGGGACACGGTGACCCACTTTGGTATTCTAACAAAATGAGTTGGTCCAAGAGTGTGATCAAGGAAGAAATGTTGATCAATCTTCATCTGGAAGGAACGTTCAATGGGCACTACTTTGAAATAAAAGGCAAAGGAAAAGGGAACCCTAATGAAGGCACCAATACCGTCACGCTCGAGGTTACCAAGGGTGGACCTCTGCCATTTGGTTGGCATATTTTGTGCCCACAATTTCAGTATGGAAACAAGGCATTTGTCCACCACCCTGACGACATACCCGATTATCTAAAGCTGTCATTTCCGGAGGGATATACATGGGAACGGTCCATGCACTTTGAAGACGGTGGCTTGTGTTGTATCACCAATGATATCAGTTTGACAGGCAACTGTTTCAACTACGACATCAAGTTCACTGGCTTGAACTTTCCTCCAAATGGACCCGTTGTGCAGAAGAAGACAACTGGCTGGGAACCGAGCACTGAGCGTTTGTATCCTCGTGATGGCGTGTTGATAGGAGACATCCATCATGCTCTCACAGTGGCAGGAGGTGGTCATTACGTATGTGACATTAAAACTGTTTACAGGGCCAAAAASCCCGTAAAGATGCCAGGGTATCACTATGTTGACCCCAAACTGGTTATAAGGAGCAACGACAAAGAATTCATGAAAGTTGAGGAGCATGAAATCGCCGTTGCACGCCNCCATCCGCTCCAAAGCCAATGAAGCTTAAGTAAAGGCAAAAAGGTGACGAGGCATGATAGTATGACATGATAGTATGACATGATAGTATGACATGATAGTAAGAATTGTAAGCAAAAGGCTTTGCTTATTAAACTTGTAATTG</t>
   </si>
 </sst>
 </file>
@@ -22792,7 +22801,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -22812,15 +22821,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -22890,7 +22890,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -22918,13 +22918,13 @@
     <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -22933,15 +22933,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
@@ -22949,6 +22947,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -22988,21 +23001,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -23569,7 +23567,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A4:I9" headerRowDxfId="21" totalsRowDxfId="18" headerRowBorderDxfId="20" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A4:I7" headerRowDxfId="21" totalsRowDxfId="18" headerRowBorderDxfId="20" tableBorderDxfId="19">
   <tableColumns count="9">
     <tableColumn id="1" name="Part Name" dataDxfId="17"/>
     <tableColumn id="16" name="SBOL Object Type" dataDxfId="16"/>
@@ -23578,7 +23576,7 @@
     <tableColumn id="5" name="Part Description" dataDxfId="13"/>
     <tableColumn id="6" name="Data Source Prefix" dataDxfId="12"/>
     <tableColumn id="7" name="Data Source" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="9" name="Sequence" dataDxfId="4"/>
+    <tableColumn id="9" name="Sequence" dataDxfId="0"/>
     <tableColumn id="13" name="Data Source Composite" dataDxfId="10">
       <calculatedColumnFormula>Library!$F5&amp;":"&amp;Library!$G5</calculatedColumnFormula>
     </tableColumn>
@@ -23828,13 +23826,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y41"/>
+  <dimension ref="A1:Y37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11:G12"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -23947,7 +23945,7 @@
       <c r="G4" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="41" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="33" t="s">
@@ -23956,7 +23954,7 @@
     </row>
     <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>7498</v>
+        <v>7500</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>7421</v>
@@ -23971,17 +23969,17 @@
         <v>7492</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="17">
-        <v>27732583</v>
+        <v>7494</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>7499</v>
       </c>
       <c r="H5" s="44" t="s">
-        <v>7495</v>
+        <v>7505</v>
       </c>
       <c r="I5" s="42" t="str">
         <f>Library!$F5&amp;":"&amp;Library!$G5</f>
-        <v>PubMed:27732583</v>
+        <v>Uniprot:Q9U6Y4</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -23998,7 +23996,7 @@
       <c r="V5" s="1"/>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="15" t="s">
         <v>7490</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -24011,24 +24009,24 @@
         <v>13</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>7493</v>
+        <v>7501</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="17">
-        <v>27732583</v>
+        <v>7494</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>7502</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>7496</v>
+        <v>7506</v>
       </c>
       <c r="I6" s="42" t="str">
         <f>Library!$F6&amp;":"&amp;Library!$G6</f>
-        <v>PubMed:27732583</v>
+        <v>Uniprot:Q8ISF8</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="15" t="s">
         <v>7491</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -24038,124 +24036,112 @@
         <v>1399</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="43" t="s">
+        <v>7503</v>
+      </c>
+      <c r="F7" s="27" t="s">
         <v>7494</v>
       </c>
-      <c r="F7" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="17">
-        <v>27732583</v>
+      <c r="G7" s="17" t="s">
+        <v>7504</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>7497</v>
+        <v>7507</v>
       </c>
       <c r="I7" s="42" t="str">
         <f>Library!$F7&amp;":"&amp;Library!$G7</f>
-        <v>PubMed:27732583</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="46" t="s">
-        <v>7499</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>7421</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>1399</v>
-      </c>
-      <c r="D8" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="47" t="s">
-        <v>7500</v>
-      </c>
-      <c r="F8" s="28"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="48" t="s">
-        <v>7503</v>
-      </c>
-      <c r="I8" s="42"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
+        <v>Uniprot:Q66ND6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
     </row>
     <row r="9" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
-        <v>7501</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>7421</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>1399</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>7502</v>
-      </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="48" t="s">
-        <v>7504</v>
-      </c>
-      <c r="I9" s="42"/>
-    </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="1"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L10" s="1"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="L11" s="1"/>
       <c r="M11" s="8"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="1"/>
+      <c r="M12" s="8"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="L13" s="1"/>
       <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L14" s="1"/>
-      <c r="M14" s="8"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="L15" s="1"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-    </row>
-    <row r="16" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="L16" s="1"/>
       <c r="M16" s="8"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="L17" s="1"/>
-      <c r="M17" s="8"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -24169,29 +24155,19 @@
       <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-    </row>
-    <row r="19" spans="12:25" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="L19" s="1"/>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="L20" s="1"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+    <row r="19" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
@@ -24203,57 +24179,55 @@
       <c r="X20" s="1"/>
       <c r="Y20" s="1"/>
     </row>
-    <row r="21" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-    </row>
-    <row r="23" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-    </row>
-    <row r="24" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-    </row>
-    <row r="26" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-      <c r="Y26" s="1"/>
-    </row>
-    <row r="32" spans="12:25" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="28" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="30" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" spans="14:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -24264,6 +24238,18 @@
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
       <c r="Y32" s="1"/>
+    </row>
+    <row r="33" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
     </row>
     <row r="34" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P34" s="1"/>
@@ -24277,18 +24263,6 @@
       <c r="X34" s="1"/>
       <c r="Y34" s="1"/>
     </row>
-    <row r="35" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-    </row>
     <row r="36" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -24312,42 +24286,6 @@
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
       <c r="Y37" s="1"/>
-    </row>
-    <row r="38" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-      <c r="Y38" s="1"/>
-    </row>
-    <row r="40" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-      <c r="Y40" s="1"/>
-    </row>
-    <row r="41" spans="16:25" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-      <c r="X41" s="1"/>
-      <c r="Y41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -24362,25 +24300,25 @@
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F9</xm:sqref>
+          <xm:sqref>F5:F7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Object_Types!$A$2:$A$35</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B9</xm:sqref>
+          <xm:sqref>B5:B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>role_terms!$B$2:$B$2518</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D9</xm:sqref>
+          <xm:sqref>D5:D7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>molecule_types!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C5:C9</xm:sqref>
+          <xm:sqref>C5:C7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25101,18 +25039,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:L2 H4:L11">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:L3">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25439,7 +25377,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25607,11 +25545,24 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="46" t="s">
+        <v>7493</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>7494</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>7496</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>7495</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>7498</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>7497</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
@@ -25669,6 +25620,9 @@
     <hyperlink ref="F7" r:id="rId17"/>
     <hyperlink ref="D3" r:id="rId18"/>
     <hyperlink ref="F8" r:id="rId19" display="https://identifiers.org/taxonomy:{REPLACE_HERE}"/>
+    <hyperlink ref="C9" r:id="rId20"/>
+    <hyperlink ref="F9" r:id="rId21"/>
+    <hyperlink ref="D9" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>